<commit_message>
Add modifications to support web element visible and assert data fetch 	modified:   app/data/platformdata.xlsx 	modified:   app/pageobject/pageobjectinfo.py 	modified:   app/pages/checkout.py 	modified:   app/test/test_checkout.py 	new file:   app/utility/assertutility.py 	modified:   app/utility/baseutility.py 	modified:   requirements.txt
</commit_message>
<xml_diff>
--- a/app/data/platformdata.xlsx
+++ b/app/data/platformdata.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soumyajitbasu/Documents/codebase/my_works/bestbuy/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6AA4FD0-9A5A-5D4C-8ED0-D4EBB1ECE93E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D650DE-8014-BE4D-ABB5-3F89BB69FD44}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{8BEB956E-017B-0D4C-8E4A-29BAB4A1E70B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="2" xr2:uid="{8BEB956E-017B-0D4C-8E4A-29BAB4A1E70B}"/>
   </bookViews>
   <sheets>
     <sheet name="customer_data" sheetId="1" r:id="rId1"/>
     <sheet name="search_keyword" sheetId="2" r:id="rId2"/>
+    <sheet name="assert_data" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>product_type</t>
   </si>
@@ -95,6 +96,18 @@
   </si>
   <si>
     <t>AB</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>search_result</t>
+  </si>
+  <si>
+    <t>Results for: EOS Rebel T7 DSLR Camera</t>
+  </si>
+  <si>
+    <t>assert_keyword</t>
   </si>
 </sst>
 </file>
@@ -459,8 +472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05F90A5B-8F67-3340-B195-7143075628B0}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -553,7 +566,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -581,4 +594,37 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A3A4904-9B32-C942-AC72-1620336B1FB1}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="74.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Make mods for taking screenshot 	modified:   app/configurations/projectconfig.json 	modified:   app/data/platformdata.xlsx 	modified:   app/pageobject/pageobjectinfo.py 	modified:   app/pages/checkout.py 	modified:   app/utility/baseutility.py 	modified:   requirements.txt
</commit_message>
<xml_diff>
--- a/app/data/platformdata.xlsx
+++ b/app/data/platformdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soumyajitbasu/Documents/codebase/my_works/bestbuy/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D650DE-8014-BE4D-ABB5-3F89BB69FD44}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E10AECC-1C40-F842-8D75-49DDEA7F84A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="2" xr2:uid="{8BEB956E-017B-0D4C-8E4A-29BAB4A1E70B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21380" activeTab="2" xr2:uid="{8BEB956E-017B-0D4C-8E4A-29BAB4A1E70B}"/>
   </bookViews>
   <sheets>
     <sheet name="customer_data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>product_type</t>
   </si>
@@ -108,13 +108,19 @@
   </si>
   <si>
     <t>assert_keyword</t>
+  </si>
+  <si>
+    <t>item_header</t>
+  </si>
+  <si>
+    <t>Canon EOS Rebel T7 DSLR Camera with 18-55mm IS Lens Kit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -126,6 +132,13 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1D252C"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -152,9 +165,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -598,9 +612,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A3A4904-9B32-C942-AC72-1620336B1FB1}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -624,6 +640,14 @@
         <v>22</v>
       </c>
     </row>
+    <row r="3" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>